<commit_message>
Switched text modeling to in-press, added dsi seed grant
</commit_message>
<xml_diff>
--- a/data/grants.xlsx
+++ b/data/grants.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Desktop/trial-cv/_cv_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/anderson-cv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7ACCA71-7301-5E45-AF2B-D02E39A48176}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00BF8A14-3AD1-DA44-9AD3-522C922B5678}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36020" yWindow="3120" windowWidth="27640" windowHeight="16940" xr2:uid="{2F3CED88-84B5-4249-9663-01EB28D3FE1D}"/>
+    <workbookView xWindow="2580" yWindow="3560" windowWidth="27640" windowHeight="16940" xr2:uid="{2F3CED88-84B5-4249-9663-01EB28D3FE1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -528,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4605E665-D6A4-C749-961B-EF6BCFDB74F3}">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5:N9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -655,7 +655,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -668,10 +668,10 @@
         <v>5</v>
       </c>
       <c r="G4" s="6">
-        <v>43831</v>
+        <v>43862</v>
       </c>
       <c r="H4" s="6">
-        <v>44196</v>
+        <v>44227</v>
       </c>
       <c r="I4">
         <v>48903.17</v>
@@ -686,7 +686,7 @@
         <v>0</v>
       </c>
       <c r="N4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added funder to grants, removed some that didn't get funded
</commit_message>
<xml_diff>
--- a/data/grants.xlsx
+++ b/data/grants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/anderson-cv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A64D827-3D75-A346-9560-EB2A9F950269}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24CCD9E1-A35A-A245-9222-F246A086B568}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34080" yWindow="7280" windowWidth="27640" windowHeight="16940" xr2:uid="{2F3CED88-84B5-4249-9663-01EB28D3FE1D}"/>
+    <workbookView xWindow="2140" yWindow="5200" windowWidth="27640" windowHeight="16940" xr2:uid="{2F3CED88-84B5-4249-9663-01EB28D3FE1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="69">
   <si>
     <t>title</t>
   </si>
@@ -229,6 +229,9 @@
   </si>
   <si>
     <t>Exploring Pathways to Desistance and Adjustment in Adulthood Among Juvenile Justice-Involved Females</t>
+  </si>
+  <si>
+    <t>omit</t>
   </si>
 </sst>
 </file>
@@ -632,7 +635,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1212,7 +1215,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="B15" s="13" t="s">
         <v>55</v>
@@ -1288,7 +1291,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="B17" s="13" t="s">
         <v>57</v>
@@ -1326,7 +1329,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="B18" s="13" t="s">
         <v>59</v>
@@ -1364,7 +1367,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="B19" s="13" t="s">
         <v>61</v>

</xml_diff>